<commit_message>
potential radiance/solid angle solution
</commit_message>
<xml_diff>
--- a/comparison/mobley_problems/Mobley_comparisons.xlsx
+++ b/comparison/mobley_problems/Mobley_comparisons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mgimond\aomc\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mgimond\aomc\comparison\mobley_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540AE111-09CA-41EC-A665-2BFF5A60F8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE9D718-6F51-4862-A137-CAE73C831CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11570" yWindow="10190" windowWidth="21960" windowHeight="12640" xr2:uid="{3BE46ACD-53F2-4C9A-9617-386117E62B42}"/>
+    <workbookView xWindow="1275" yWindow="7200" windowWidth="23580" windowHeight="8235" xr2:uid="{3BE46ACD-53F2-4C9A-9617-386117E62B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,15 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Mobley 1  s/(a+s) =0.2</t>
   </si>
@@ -81,13 +84,19 @@
   </si>
   <si>
     <t>AOMC</t>
+  </si>
+  <si>
+    <t>AMC</t>
+  </si>
+  <si>
+    <t>Relative difference (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,9 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,22 +471,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64285B62-72D9-4F0B-92B8-DCDE774A5D1B}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="5" max="6" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -485,8 +499,14 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -514,13 +534,22 @@
       <c r="K2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>0.8</v>
       </c>
@@ -542,17 +571,29 @@
       <c r="G4" s="1">
         <v>1.72E-3</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>1E-3</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M4" s="2">
+        <f>(E4-B4)/E4</f>
+        <v>-3.7021276595746275E-3</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N6" si="0">(F4-C4)/F4</f>
+        <v>8.5820895522388443E-3</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O6" si="1">(G4-D4)/G4</f>
+        <v>8.1395348837208763E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -560,7 +601,7 @@
         <v>1.07E-3</v>
       </c>
       <c r="C5">
-        <v>9.2E-5</v>
+        <v>9.7999999999999997E-5</v>
       </c>
       <c r="D5">
         <v>1.34E-5</v>
@@ -574,17 +615,29 @@
       <c r="G5" s="1">
         <v>1.3699999999999999E-5</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <v>3.9E-2</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2">
         <v>0.28799999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M5" s="2">
+        <f>(E5-B5)/E5</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="0"/>
+        <v>2.000000000000008E-2</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1897810218978016E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>8</v>
       </c>
@@ -606,33 +659,48 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>0.10199999999999999</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <v>0.308</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="2">
         <v>0.19700000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M6" s="2">
+        <f>(E6-B6)/E6</f>
+        <v>-2.3890784982935214E-2</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>0.1</v>
       </c>
       <c r="B8">
-        <v>0.36593799999999999</v>
+        <v>0.36600500000000002</v>
       </c>
       <c r="C8">
-        <v>0.37189899999999998</v>
+        <v>0.37022699999999997</v>
       </c>
       <c r="D8">
-        <v>4.8563200000000001E-2</v>
+        <v>4.8825E-2</v>
       </c>
       <c r="E8" s="1">
         <v>0.36599999999999999</v>
@@ -643,28 +711,40 @@
       <c r="G8" s="1">
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>2E-3</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M8" s="2">
+        <f>(E8-B8)/E8</f>
+        <v>-1.3661202185881847E-5</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" ref="N8:N10" si="2">(F8-C8)/F8</f>
+        <v>4.7661290322581302E-3</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" ref="O8:O10" si="3">(G8-D8)/G8</f>
+        <v>-6.7010309278350286E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>0.5</v>
       </c>
       <c r="B9">
-        <v>4.3289000000000001E-2</v>
+        <v>4.3282000000000001E-2</v>
       </c>
       <c r="C9">
-        <v>4.6199999999999998E-2</v>
+        <v>4.3249999999999997E-2</v>
       </c>
       <c r="D9">
-        <v>5.8069999999999997E-3</v>
+        <v>5.7650000000000002E-3</v>
       </c>
       <c r="E9" s="1">
         <v>4.3299999999999998E-2</v>
@@ -675,28 +755,40 @@
       <c r="G9" s="1">
         <v>5.5900000000000004E-3</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="2">
         <v>5.1999999999999998E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M9" s="2">
+        <f>(E9-B9)/E9</f>
+        <v>4.1570438799069711E-4</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>5.7471264367816143E-3</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="3"/>
+        <v>-3.1305903398926617E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>3.1470000000000001E-3</v>
+        <v>3.1419999999999998E-3</v>
       </c>
       <c r="C10">
-        <v>3.1510000000000002E-3</v>
+        <v>3.1340000000000001E-3</v>
       </c>
       <c r="D10">
-        <v>4.0529999999999999E-4</v>
+        <v>4.2499999999999998E-4</v>
       </c>
       <c r="E10" s="1">
         <v>3.16E-3</v>
@@ -707,33 +799,53 @@
       <c r="G10" s="1">
         <v>4.37E-4</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="2">
         <v>9.0999999999999998E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M10" s="2">
+        <f>(E10-B10)/E10</f>
+        <v>5.696202531645639E-3</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>2.0625000000000025E-2</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="3"/>
+        <v>2.7459954233409658E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>0.8</v>
       </c>
       <c r="B13">
-        <v>0.16206799999999999</v>
+        <v>0.161871985</v>
       </c>
       <c r="C13">
-        <v>9.7400000000000004E-4</v>
+        <v>9.91949E-4</v>
       </c>
       <c r="D13">
-        <v>6.7799999999999995E-5</v>
+        <v>5.2506000000000002E-5</v>
       </c>
       <c r="E13" s="1">
         <v>0.16200000000000001</v>
@@ -744,28 +856,40 @@
       <c r="G13" s="1">
         <v>5.4700000000000001E-5</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>0</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="2">
         <v>2.3E-2</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="2">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M13" s="2">
+        <f>(E13-B13)/E13</f>
+        <v>7.9021604938277212E-4</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" ref="N13:N15" si="4">(F13-C13)/F13</f>
+        <v>-2.6862318840579758E-2</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" ref="O13:O15" si="5">(G13-D13)/G13</f>
+        <v>4.0109689213893962E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>4</v>
       </c>
       <c r="B14">
-        <v>2.2850000000000001E-3</v>
+        <v>2.2633530000000001E-3</v>
       </c>
       <c r="C14">
-        <v>1.4E-5</v>
+        <v>1.2683E-5</v>
       </c>
       <c r="D14">
-        <v>7.9999999999999996E-7</v>
+        <v>7.37E-7</v>
       </c>
       <c r="E14" s="1">
         <v>2.2699999999999999E-3</v>
@@ -776,65 +900,93 @@
       <c r="G14" s="1">
         <v>6.2399999999999998E-7</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>2E-3</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="2">
         <v>6.3E-2</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="2">
         <v>0.35499999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M14" s="2">
+        <f>(E14-B14)/E14</f>
+        <v>2.9281938325990383E-3</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="4"/>
+        <v>7.4233576642335694E-2</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="5"/>
+        <v>-0.18108974358974364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>8</v>
       </c>
       <c r="B15">
-        <v>1.2999999999999999E-5</v>
+        <v>1.3200000000000001E-5</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>8.0000000000000002E-8</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2E-8</v>
       </c>
       <c r="E15" s="1">
         <v>1.2999999999999999E-5</v>
       </c>
-      <c r="F15" s="1">
-        <v>0</v>
+      <c r="F15" s="3">
+        <v>7.2800000000000003E-8</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15">
+        <f>0.00000000402</f>
+        <v>4.0199999999999998E-9</v>
+      </c>
+      <c r="I15" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="2">
         <v>0.187</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="2">
         <v>0.248</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M15" s="2">
+        <f>(E15-B15)/E15</f>
+        <v>-1.5384615384615498E-2</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="4"/>
+        <v>-9.8901098901098869E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="5"/>
+        <v>-3.9751243781094532</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>0.1</v>
       </c>
       <c r="B17">
-        <v>0.41350700000000001</v>
+        <v>0.4135972</v>
       </c>
       <c r="C17">
-        <v>9.3312000000000006E-2</v>
+        <v>9.0251239999999996E-2</v>
       </c>
       <c r="D17">
-        <v>7.0737999999999999E-3</v>
+        <v>7.8971800000000002E-3</v>
       </c>
       <c r="E17" s="1">
         <v>0.41299999999999998</v>
@@ -845,28 +997,40 @@
       <c r="G17" s="1">
         <v>6.9899999999999997E-3</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="2">
         <v>1E-3</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="2">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="2">
         <v>6.3E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M17" s="2">
+        <f>(E17-B17)/E17</f>
+        <v>-1.4460048426150605E-3</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" ref="N17:N19" si="6">(F17-C17)/F17</f>
+        <v>3.0598925886143991E-2</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" ref="O17:O19" si="7">(G17-D17)/G17</f>
+        <v>-0.12978254649499293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>0.5</v>
       </c>
       <c r="B18">
-        <v>0.18729899999999999</v>
+        <v>0.183851182</v>
       </c>
       <c r="C18">
-        <v>4.6185999999999998E-2</v>
+        <v>4.7438267999999999E-2</v>
       </c>
       <c r="D18">
-        <v>3.1966999999999998E-3</v>
+        <v>3.3217899999999998E-3</v>
       </c>
       <c r="E18" s="1">
         <v>0.187</v>
@@ -877,28 +1041,40 @@
       <c r="G18" s="1">
         <v>3.29E-3</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="2">
         <v>5.5E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M18" s="2">
+        <f>(E18-B18)/E18</f>
+        <v>1.6838598930481272E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="6"/>
+        <v>-2.4584622030237535E-2</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="7"/>
+        <v>-9.6626139817628746E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19">
-        <v>6.8703E-2</v>
+        <v>6.6183403000000002E-2</v>
       </c>
       <c r="C19">
-        <v>1.6323000000000001E-2</v>
+        <v>1.6484321999999999E-2</v>
       </c>
       <c r="D19">
-        <v>1.1839999999999999E-3</v>
+        <v>1.1833119999999999E-3</v>
       </c>
       <c r="E19" s="1">
         <v>6.8500000000000005E-2</v>
@@ -909,22 +1085,37 @@
       <c r="G19" s="1">
         <v>1.2099999999999999E-3</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="2">
         <v>0.01</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="2">
         <v>1.4E-2</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="2">
         <v>0.109</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M19" s="2">
+        <f>(E19-B19)/E19</f>
+        <v>3.381893430656939E-2</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="6"/>
+        <v>9.5018181818191559E-4</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="7"/>
+        <v>2.2056198347107415E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -939,17 +1130,17 @@
         <f>3.13*10^-3</f>
         <v>3.13E-3</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="2">
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -965,17 +1156,17 @@
         <f>2.12*10^-5</f>
         <v>2.1200000000000004E-5</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="2">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="2">
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -991,33 +1182,36 @@
         <f>3.57*10^-7</f>
         <v>3.5699999999999998E-7</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="2">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="2">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="2">
         <v>0.434</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25">
         <v>0.8</v>
       </c>
       <c r="B25">
-        <v>0.16203999999999999</v>
+        <v>0.16184699999999999</v>
       </c>
       <c r="C25">
-        <v>1E-3</v>
+        <v>1.0089999999999999E-3</v>
       </c>
       <c r="D25">
-        <v>7.5599999999999994E-5</v>
+        <v>6.8999999999999997E-5</v>
       </c>
       <c r="E25" s="1">
         <v>0.16200000000000001</v>
@@ -1030,28 +1224,40 @@
         <f>6.84*10^-5</f>
         <v>6.8400000000000009E-5</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="2">
         <v>0</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="2">
         <v>0.01</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="2">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M25" s="2">
+        <f>(E25-B25)/E25</f>
+        <v>9.444444444445323E-4</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" ref="N25:O25" si="8">(F25-C25)/F25</f>
+        <v>-2.8437468147997122E-2</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="8"/>
+        <v>-8.7719298245612191E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26">
-        <v>2.2859999999999998E-3</v>
+        <v>2.2669999999999999E-3</v>
       </c>
       <c r="C26">
-        <v>2.2889999999999998E-3</v>
+        <v>2.2669999999999999E-3</v>
       </c>
       <c r="D26">
-        <v>3.6620000000000001E-4</v>
+        <v>3.6099999999999999E-4</v>
       </c>
       <c r="E26" s="1">
         <f>2.28*10^-3</f>
@@ -1065,17 +1271,30 @@
         <f>3.6*10^-4</f>
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="2">
         <v>2E-3</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="2">
         <v>0.01</v>
+      </c>
+      <c r="M26" s="2">
+        <f>(E26-B26)/E26</f>
+        <v>5.7017543859649083E-3</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" ref="N26" si="9">(F26-C26)/F26</f>
+        <v>5.7017543859649083E-3</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" ref="O26" si="10">(G26-D26)/G26</f>
+        <v>-2.7777777777776946E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>